<commit_message>
added some input checking
</commit_message>
<xml_diff>
--- a/example/requests.xlsx
+++ b/example/requests.xlsx
@@ -796,10 +796,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>32</v>
@@ -817,10 +817,10 @@
         <v>32</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>

</xml_diff>